<commit_message>
2 hubs and 1/2 link
</commit_message>
<xml_diff>
--- a/Modelling.xlsx
+++ b/Modelling.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevec\PycharmProjects\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BF1EC3-7073-4709-9A80-F349A7DBB395}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC0FDAB-1B14-4335-A42D-7193E4EB66F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{49A5625A-624D-458B-B43F-E5DD32A9C8DB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{49A5625A-624D-458B-B43F-E5DD32A9C8DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Full_Facts" sheetId="1" r:id="rId1"/>
     <sheet name="DimTour" sheetId="2" r:id="rId2"/>
     <sheet name="DimPlayer" sheetId="3" r:id="rId3"/>
     <sheet name="DimDraw" sheetId="6" r:id="rId4"/>
-    <sheet name="Tour_Hub" sheetId="4" r:id="rId5"/>
-    <sheet name="Player_Hub" sheetId="5" r:id="rId6"/>
+    <sheet name="H_TOURN" sheetId="4" r:id="rId5"/>
+    <sheet name="S_TOUR" sheetId="7" r:id="rId6"/>
+    <sheet name="H_PLAYER" sheetId="5" r:id="rId7"/>
+    <sheet name="S_PLAYER" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Full_Facts!$A$1:$B$49</definedName>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
   <si>
     <t>tourney_id</t>
   </si>
@@ -596,11 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A51957-2014-414D-8EAC-38B406E417AC}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,7 +618,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -625,7 +626,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -633,7 +634,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -641,7 +642,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -649,7 +650,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -657,7 +658,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -670,12 +671,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -728,12 +729,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -778,7 +779,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -786,7 +787,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -794,7 +795,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -802,7 +803,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -810,7 +811,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -818,7 +819,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -826,7 +827,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -834,7 +835,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -842,7 +843,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -850,7 +851,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -858,7 +859,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -866,7 +867,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -874,7 +875,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -882,7 +883,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -890,7 +891,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -898,7 +899,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -906,7 +907,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -914,7 +915,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -922,7 +923,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -930,7 +931,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -938,7 +939,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -946,7 +947,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -954,7 +955,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -962,7 +963,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -970,7 +971,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -978,7 +979,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -987,13 +988,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B49" xr:uid="{E3CC53AA-C591-43BF-A674-7222BB5EAA7A}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="DimPlayer"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:B49" xr:uid="{E3CC53AA-C591-43BF-A674-7222BB5EAA7A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1002,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2355C36D-B954-4F19-A94F-26D67E2CEE9E}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1220,7 +1215,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1262,6 +1257,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6E6322-F188-444E-8405-638CAE14CE02}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E027AA-0F7B-4BC5-B015-E2B44EC5549F}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1272,7 +1302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F29895-BFDB-4292-9967-672A63534EC1}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1282,4 +1312,18 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFC21F9F-9F5E-4F93-8044-D9EC076A6CD5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>